<commit_message>
Updated test cases and bug report templates
</commit_message>
<xml_diff>
--- a/FunctionalTesting+BugReporting_Task1.xlsx
+++ b/FunctionalTesting+BugReporting_Task1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stoqn\Desktop\SoftUni\QA Fundamentals and Manual Testing\ExamPrep1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\MyProjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5053BF-5DBF-4264-B112-E97312C08CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F709B8B3-B651-43CC-B8A7-F5EFE4953086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25840" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Use Case 1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="265">
   <si>
     <t>Expected result:</t>
   </si>
@@ -163,11 +163,6 @@
     <t>Spelling mistakes on the carousel on the home page for not-logged in users</t>
   </si>
   <si>
-    <t>1.to have a slide with text: 
--Enjoy our site!
--Be part of our community</t>
-  </si>
-  <si>
     <t>Fail</t>
   </si>
   <si>
@@ -197,9 +192,6 @@
     <t>Wrong text of navigation button for SIGN IN</t>
   </si>
   <si>
-    <t>The button for sign in the systen should have "SIGN IN" text</t>
-  </si>
-  <si>
     <t>The button for sign in the system have "LOGIN" as text</t>
   </si>
   <si>
@@ -217,9 +209,6 @@
     <t>UC1-4</t>
   </si>
   <si>
-    <t>Wrong text of carousel button for SIGN UP FOR FREE</t>
-  </si>
-  <si>
     <t>The button SIGN UP FOR FREE in the coursel have "REGISTER NOW"as text</t>
   </si>
   <si>
@@ -232,15 +221,6 @@
   <si>
     <t>1. Open application URL.
 2. Loggin with the registered user.</t>
-  </si>
-  <si>
-    <t>Verify the carousel have the correct sections/slides: 
--Welcome to idea Center USER
--See your profil
--See your ideas</t>
-  </si>
-  <si>
-    <t>User is correctly navigated when click different buttons</t>
   </si>
   <si>
     <t>UC1-1</t>
@@ -381,24 +361,9 @@
     <t>UC2-6</t>
   </si>
   <si>
-    <t>Verify user cannot be registrered with email below the constraints</t>
-  </si>
-  <si>
     <t>UC2-7</t>
   </si>
   <si>
-    <t>Verify user cannot be registrered with email above the constraints</t>
-  </si>
-  <si>
-    <t>Verify user cannot be registrered with password below the constraints</t>
-  </si>
-  <si>
-    <t>Verify user cannot be registrered with password above the constraints</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify user cannot be registrered with not matching password </t>
-  </si>
-  <si>
     <t>UC2-8</t>
   </si>
   <si>
@@ -409,15 +374,6 @@
   </si>
   <si>
     <t>UC2-11</t>
-  </si>
-  <si>
-    <t>Verify user cannot be registrered without accepting the terms</t>
-  </si>
-  <si>
-    <t>UC2-12</t>
-  </si>
-  <si>
-    <t>Veirfy user is registered with all vaild data</t>
   </si>
   <si>
     <t>UC3-1</t>
@@ -539,22 +495,6 @@
   <si>
     <t>1. Click my profil button.
 2. Click edit profile
-3. Fill firstname with more than 60 characters
-4. Fill valid lastname
-5. Fill valid city
-6. Fill valid description</t>
-  </si>
-  <si>
-    <t>1. Click my profil button.
-2. Click edit profile
-3. Fill valid firstname 
-4. Fill lastname with more than 60 characters
-5. Fill valid city
-6. Fill valid description</t>
-  </si>
-  <si>
-    <t>1. Click my profil button.
-2. Click edit profile
 3. Fill valid firstname 
 4. Fill valid lastname 
 5. Fill city with more than 120 characters
@@ -584,9 +524,6 @@
     <t>Medium</t>
   </si>
   <si>
-    <t>When user edit text with values with max characters for last name and city the data is not displayed correctly</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Log into the system
 2. Click my profil
 3. Click etid profil
@@ -617,18 +554,12 @@
     <t>User cannot create idea with 2 chars as title</t>
   </si>
   <si>
-    <t>The idea is not created</t>
-  </si>
-  <si>
     <t>BGID-7</t>
   </si>
   <si>
     <t>User can create idea with title with 2 chars</t>
   </si>
   <si>
-    <t>The idea is not created. Error message is displayed</t>
-  </si>
-  <si>
     <t>The idea is not created. Error message is displayed.</t>
   </si>
   <si>
@@ -713,13 +644,381 @@
     <t>BGID-9</t>
   </si>
   <si>
-    <t>UC6-5/6</t>
-  </si>
-  <si>
     <t>Blocking</t>
   </si>
   <si>
     <t>When users performs search by keyword the application crashes</t>
+  </si>
+  <si>
+    <t>1. To have a slide with text: 
+-Enjoy our site!
+-Be part of our community</t>
+  </si>
+  <si>
+    <t>The button for sign in the system should have "SIGN IN" text</t>
+  </si>
+  <si>
+    <t>Wrong text of carousel button for "SIGN UP FOR FREE"</t>
+  </si>
+  <si>
+    <t>User is not logged in</t>
+  </si>
+  <si>
+    <t>Verify SIGN IN button from Navigation bar</t>
+  </si>
+  <si>
+    <t>1. Open the application URL.
+2. Click on SIGN IN button from upper-right part in the NavBar</t>
+  </si>
+  <si>
+    <t>SIGN IN page is loaded</t>
+  </si>
+  <si>
+    <t>Verify SIGN IN button from Carousel</t>
+  </si>
+  <si>
+    <t>1. Open the application URL.
+2. Click on SIGN IN button from the Carousel</t>
+  </si>
+  <si>
+    <t>Verify SIGN UP FOR FREE button from Navigation bar</t>
+  </si>
+  <si>
+    <t>1. Open the application URL.
+2. Click on SIGN UP FOR FREE button from upper-right part in the NavBar</t>
+  </si>
+  <si>
+    <t>SIGN UP FOR FREE page is loaded</t>
+  </si>
+  <si>
+    <t>Verify SIGN UP FOR FREE button from Carousel</t>
+  </si>
+  <si>
+    <t>1. Open the application URL.
+2. Click on SIGN UP FOR FREE button from the Carousel</t>
+  </si>
+  <si>
+    <t>Registered user is existing</t>
+  </si>
+  <si>
+    <t>Verify the carousel with logged in user</t>
+  </si>
+  <si>
+    <t>1. Open the application URL.
+2. Login with user</t>
+  </si>
+  <si>
+    <t>Verify the carousel displays following three slides:
+-Welcome to Idea Center, User
+-Control your own idea space
+-Enjoy your space for ideas</t>
+  </si>
+  <si>
+    <t>UC1-11</t>
+  </si>
+  <si>
+    <t>Verify the Navigation bar with logged in user</t>
+  </si>
+  <si>
+    <t>The following button/links are present:
+- My Profile link ;
+- My Ideas link ;
+- Create Ideas link;
+- Logout button;</t>
+  </si>
+  <si>
+    <t>Verify registration with Email below the lower boundary</t>
+  </si>
+  <si>
+    <t>1. Open the application.
+2. Click on SIGNUP FOR FREE button.
+3. Enter for username "AAA".
+4. Enter email "a@a.a".
+5. Enter password and repeat password - "123456".
+6. Click on 'SIN UP" button,</t>
+  </si>
+  <si>
+    <t>Validation message for Email should appears</t>
+  </si>
+  <si>
+    <t>Lower boundary for Email filed is 6 symbols</t>
+  </si>
+  <si>
+    <t>Verify registration with Email on the lower boundary</t>
+  </si>
+  <si>
+    <t>1. Open the application.
+2. Click on SIGNUP FOR FREE button.
+3. Enter for username "AAA".
+4. Enter email "a@a.aa".
+5. Enter password and repeat password - "123456".
+6. Select the checkbox to accept terms and services.
+7. Click on 'SIN UP" button.</t>
+  </si>
+  <si>
+    <t>User is successfully registered.</t>
+  </si>
+  <si>
+    <t>Verify registration with Email on the upper boundary</t>
+  </si>
+  <si>
+    <t>1. Open the application.
+2. Click on SIGNUP FOR FREE button.
+3. Enter for username "AAA".
+4. Enter email with 254 symbol length.
+5. Enter password and repeat password - "123456".
+6. Select the checkbox to accept terms and services.
+7. Click on 'SIN UP" button.</t>
+  </si>
+  <si>
+    <t>Upper boundary for Email filed is 254 symbols</t>
+  </si>
+  <si>
+    <t>Verify registration with Paasword below the lower boundary</t>
+  </si>
+  <si>
+    <t>1. Open the application.
+2. Click on SIGNUP FOR FREE button.
+3. Enter for username "AAA".
+4. Enter email "test@test.bg".
+5. Enter password and repeat password - "12345".
+6. Click on 'SIN UP" button,</t>
+  </si>
+  <si>
+    <t>Validation message for Password should appears</t>
+  </si>
+  <si>
+    <t>Lower boundary for Password filed is 6 symbols</t>
+  </si>
+  <si>
+    <t>Verify registration with Password on the lower boundary</t>
+  </si>
+  <si>
+    <t>1. Open the application.
+2. Click on SIGNUP FOR FREE button.
+3. Enter for username "AAA".
+4. Enter email "test@test.bg".
+5. Enter password and repeat password - "123456".
+6. Select the checkbox to accept terms and services.
+7. Click on 'SIN UP" button.</t>
+  </si>
+  <si>
+    <t>Verify registration with Password on the upper boundary</t>
+  </si>
+  <si>
+    <t>1. Open the application.
+2. Click on SIGNUP FOR FREE button.
+3. Enter for username "AAA".
+4. Enter email "test@test.bg".
+5. Enter password and repeat password with 30 symbols.
+6. Select the checkbox to accept terms and services.
+7. Click on 'SIN UP" button.</t>
+  </si>
+  <si>
+    <t>Upper boundary for Password filed is 30 symbols</t>
+  </si>
+  <si>
+    <t>1. Open the application.
+2. Click on 'SIGN IN" button.
+3. Enter valid email
+4. Enter valid password
+5. Click on SIGN IN button.</t>
+  </si>
+  <si>
+    <t>Try to login with non-existing user and empty password</t>
+  </si>
+  <si>
+    <t>Validation message for wrong username and password appears</t>
+  </si>
+  <si>
+    <t>UC3-5</t>
+  </si>
+  <si>
+    <t>1. Open the application.
+2. Click on 'SIGN IN" button.
+3. Enter not valid email and empty password
+4. Click on SIGN IN button.</t>
+  </si>
+  <si>
+    <t>The field FirstName is restricted to 60 characters</t>
+  </si>
+  <si>
+    <t>The field LastName is restricted to 60 characters</t>
+  </si>
+  <si>
+    <t>1. Click my profil button.
+2. Click edit profile
+3. Fill valid FirstName 
+4. Fill LastName with more than 60 characters
+5. Fill valid city
+6. Fill valid description</t>
+  </si>
+  <si>
+    <t>1. Click my profil button.
+2. Click edit profile
+3. Fill FirstName with more than 60 characters
+4. Fill valid LastName
+5. Fill valid city
+6. Fill valid description</t>
+  </si>
+  <si>
+    <t>Verify My Profile Page labels</t>
+  </si>
+  <si>
+    <t>Verify the following state of the form:
+- a default empty profile picture is shown;
+- Edit profile button is present;
+- Empty about section;
+- Ideas counter equal to 0;</t>
+  </si>
+  <si>
+    <t>Verify My Ideas Page labels</t>
+  </si>
+  <si>
+    <t>No ideas are shown. A message with label "No Ideas yet!" is displayed. Above the message there should be search field.</t>
+  </si>
+  <si>
+    <t>Verify Create Idea Page labels</t>
+  </si>
+  <si>
+    <t>A page for create of new idea should be opened. Following fields should be displayed:
+ - Ttile;
+ - Picture;
+ - Description</t>
+  </si>
+  <si>
+    <t>UC4-8</t>
+  </si>
+  <si>
+    <t>UC4-9</t>
+  </si>
+  <si>
+    <t>UC4-10</t>
+  </si>
+  <si>
+    <t>1. Login with valid Username and password
+2. Click on 'My Profile' link</t>
+  </si>
+  <si>
+    <t>1. Click on Create Idea.
+2.  Fill "AA" as a title.
+3. Add valid picture.
+4. Fill valid description</t>
+  </si>
+  <si>
+    <t>1. Click on Create Idea.
+2.  Fill valid title.
+3. Add valid picture.
+4. Fill description with not valid data (96 characters)</t>
+  </si>
+  <si>
+    <t>1. Click on Create Idea.
+2.  Fill valid title.
+3. Add valid picture.
+4. Fill description with not valid data (2 characters)</t>
+  </si>
+  <si>
+    <t>The description field is restricted to 400 characters.</t>
+  </si>
+  <si>
+    <t>The idea is created and user is redirected to my ideas page</t>
+  </si>
+  <si>
+    <t>All ideas are displayed on My Profile Page</t>
+  </si>
+  <si>
+    <t>1. Click on My Ideas.</t>
+  </si>
+  <si>
+    <t>All ideas are displayed on My Profile Page and have the following buttons:
+-VIEW
+-EDIT
+-DELETE</t>
+  </si>
+  <si>
+    <t>1. Click on My Ideas.
+2. Click VIEW button on an idea
+3. Click EDIT button on an idea
+4. Click DELETE button on an idea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is redirected to the idea details page
+2. User is redirected to idea Edit Page
+3. The idea is deleted successfully </t>
+  </si>
+  <si>
+    <t>The following message is displayed: No Ideas yet!</t>
+  </si>
+  <si>
+    <t>When user edit text with values with max characters for last name and city, the data is not displayed correctly</t>
+  </si>
+  <si>
+    <t>The field is restricted to 120 characters. The name of the city is positioned correctly and visible.</t>
+  </si>
+  <si>
+    <t>The field is restricted to 256 characters. The name of the city is positioned correctly and visible.</t>
+  </si>
+  <si>
+    <t>1. Click on My Ideas.
+2. Enter the name of an idea in the search field</t>
+  </si>
+  <si>
+    <t>The matching idea is displeyd.</t>
+  </si>
+  <si>
+    <t>1. Click on My Ideas.
+2. Enter a keyword that doesn’t match any of my ideas</t>
+  </si>
+  <si>
+    <t>A 'no matching results' message is displayed.</t>
+  </si>
+  <si>
+    <t>1. Click on Create Idea.
+2.  Fill valid title.
+3. Add valid picture.
+4. Fill valid description
+5. Click "CREATE" button</t>
+  </si>
+  <si>
+    <t>Logged in user. Idea is created.</t>
+  </si>
+  <si>
+    <t>1. Click on My profile</t>
+  </si>
+  <si>
+    <t>1. Click on Create Idea.
+2.  Fill valid title.
+3. Add valid picture.
+4. Fill valid description
+5. Click "CREATE" button
+6. Click on My profile</t>
+  </si>
+  <si>
+    <t>The counter displayes the number of my ideas.</t>
+  </si>
+  <si>
+    <t>The counter is not working. Always 0 ideas are displayed.</t>
+  </si>
+  <si>
+    <t>The counter displays the number of my ideas.</t>
+  </si>
+  <si>
+    <t>UC6-4/5</t>
+  </si>
+  <si>
+    <t>1. Log into the system
+2. Click on my ideas
+3. Enter any name in the se arch field
+5. Click Search button</t>
+  </si>
+  <si>
+    <t>The matching results are displayed or a 'no matching results' message is displayed.</t>
+  </si>
+  <si>
+    <t>The application crashes after clicking the button Search.</t>
+  </si>
+  <si>
+    <t>UC2-1/2</t>
   </si>
 </sst>
 </file>
@@ -903,11 +1202,11 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF5F6368"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1124,7 +1423,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1287,9 +1586,6 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1305,9 +1601,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1318,6 +1611,26 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2845,7 +3158,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{77E3F8AE-34C0-48C0-B1F8-25014EBF98C4}" name="Table_134512" displayName="Table_134512" ref="A3:G24" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{77E3F8AE-34C0-48C0-B1F8-25014EBF98C4}" name="Table_134512" displayName="Table_134512" ref="A3:G25" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{596E79C9-8B6C-4BA5-B323-4B28E49EF1BD}" name="Test Case ID" dataDxfId="46"/>
     <tableColumn id="3" xr3:uid="{E3029210-671C-4C13-B603-41C7845ED7B5}" name="Prequisites" dataDxfId="45"/>
@@ -3186,7 +3499,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15:G15"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3202,25 +3515,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
       <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" s="5" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3249,7 +3562,7 @@
     </row>
     <row r="4" spans="1:16" s="52" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B4" s="49" t="s">
         <v>36</v>
@@ -3286,70 +3599,70 @@
         <v>35</v>
       </c>
       <c r="F5" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="51" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="6" spans="1:16" s="32" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="61" t="s">
-        <v>46</v>
+      <c r="A6" s="60" t="s">
+        <v>45</v>
       </c>
       <c r="B6" s="49" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="49" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="54" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="51" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="7" spans="1:16" s="32" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="61" t="s">
-        <v>53</v>
+      <c r="A7" s="60" t="s">
+        <v>51</v>
       </c>
       <c r="B7" s="49" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D7" s="49" t="s">
         <v>33</v>
       </c>
       <c r="E7" s="51" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F7" s="54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" s="51" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="32" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="61" t="s">
-        <v>62</v>
+      <c r="A8" s="60" t="s">
+        <v>57</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C8" s="51" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="49" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E8" s="49" t="s">
         <v>29</v>
@@ -3359,104 +3672,134 @@
       </c>
       <c r="G8" s="51"/>
     </row>
-    <row r="9" spans="1:16" s="33" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="49" t="s">
+    <row r="9" spans="1:16" s="33" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="B9" s="68" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="68" t="s">
+        <v>181</v>
+      </c>
+      <c r="E9" s="68" t="s">
+        <v>182</v>
+      </c>
+      <c r="F9" s="69" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="51"/>
+    </row>
+    <row r="10" spans="1:16" s="33" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="50"/>
-      <c r="G9" s="51"/>
-    </row>
-    <row r="10" spans="1:16" s="33" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="61" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="51"/>
-      <c r="F10" s="50"/>
+      <c r="B10" s="68" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10" s="68" t="s">
+        <v>184</v>
+      </c>
+      <c r="E10" s="68" t="s">
+        <v>182</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="G10" s="51"/>
     </row>
-    <row r="11" spans="1:16" s="33" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="61" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="51"/>
-      <c r="F11" s="50"/>
+    <row r="11" spans="1:16" s="33" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="67" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="68" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" s="68" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="68" t="s">
+        <v>186</v>
+      </c>
+      <c r="E11" s="68" t="s">
+        <v>187</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="G11" s="50"/>
     </row>
     <row r="12" spans="1:16" s="33" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="61" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
+      <c r="A12" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="68" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>188</v>
+      </c>
+      <c r="D12" s="68" t="s">
+        <v>189</v>
+      </c>
+      <c r="E12" s="68" t="s">
+        <v>187</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="G12" s="50"/>
     </row>
-    <row r="13" spans="1:16" s="33" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
+    <row r="13" spans="1:16" s="33" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="68" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="68" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="68" t="s">
+        <v>192</v>
+      </c>
+      <c r="E13" s="68" t="s">
+        <v>193</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="G13" s="50"/>
     </row>
-    <row r="14" spans="1:16" s="33" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="61"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
+    <row r="14" spans="1:16" s="33" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="67" t="s">
+        <v>194</v>
+      </c>
+      <c r="B14" s="68" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>195</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>192</v>
+      </c>
+      <c r="E14" s="68" t="s">
+        <v>196</v>
+      </c>
+      <c r="F14" s="69" t="s">
+        <v>30</v>
+      </c>
       <c r="G14" s="50"/>
     </row>
     <row r="15" spans="1:16" s="33" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="61"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="51"/>
       <c r="C15" s="50"/>
       <c r="D15" s="50"/>
@@ -3465,7 +3808,7 @@
       <c r="G15" s="50"/>
     </row>
     <row r="16" spans="1:16" s="33" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="61"/>
+      <c r="A16" s="60"/>
       <c r="B16" s="51"/>
       <c r="C16" s="50"/>
       <c r="D16" s="50"/>
@@ -3474,7 +3817,7 @@
       <c r="G16" s="50"/>
     </row>
     <row r="17" spans="1:7" s="33" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="61"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="51"/>
       <c r="C17" s="50"/>
       <c r="D17" s="50"/>
@@ -3483,7 +3826,7 @@
       <c r="G17" s="50"/>
     </row>
     <row r="18" spans="1:7" s="33" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="61"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="51"/>
       <c r="C18" s="50"/>
       <c r="D18" s="50"/>
@@ -3517,11 +3860,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6991B6E1-347E-4CF1-96F5-0EDD13AED6E1}">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3536,25 +3879,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="78"/>
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="73"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="75"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="81"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" ht="28.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3581,303 +3924,354 @@
       </c>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="30"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
+    <row r="4" spans="1:16" ht="145" x14ac:dyDescent="0.35">
+      <c r="A4" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>70</v>
+      </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="30"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
+    <row r="5" spans="1:16" ht="145" x14ac:dyDescent="0.35">
+      <c r="A5" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>70</v>
+      </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="30"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+    <row r="6" spans="1:16" ht="116" x14ac:dyDescent="0.35">
+      <c r="A6" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="23"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="30"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-    </row>
-    <row r="8" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="30"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-    </row>
-    <row r="9" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="30"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-    </row>
-    <row r="10" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="30"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-    </row>
-    <row r="11" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="30"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-    </row>
-    <row r="12" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="30"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-    </row>
-    <row r="13" spans="1:16" s="7" customFormat="1" ht="145" x14ac:dyDescent="0.35">
-      <c r="A13" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" s="7" customFormat="1" ht="145" x14ac:dyDescent="0.35">
-      <c r="A14" s="24" t="s">
+    <row r="7" spans="1:16" ht="116" x14ac:dyDescent="0.35">
+      <c r="A7" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" s="7" customFormat="1" ht="116" x14ac:dyDescent="0.35">
-      <c r="A15" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="23" t="s">
+      <c r="E7" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" spans="1:16" ht="116" x14ac:dyDescent="0.35">
+      <c r="A8" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="F15" s="23" t="s">
+      <c r="E8" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="23"/>
-    </row>
-    <row r="16" spans="1:16" s="7" customFormat="1" ht="116" x14ac:dyDescent="0.35">
-      <c r="A16" s="24" t="s">
+      <c r="G8" s="23"/>
+    </row>
+    <row r="9" spans="1:16" ht="87" x14ac:dyDescent="0.35">
+      <c r="A9" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="62" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16" s="23" t="s">
+      <c r="B11" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="F11" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="23"/>
-    </row>
-    <row r="17" spans="1:7" s="7" customFormat="1" ht="116" x14ac:dyDescent="0.35">
-      <c r="A17" s="24" t="s">
+      <c r="G11" s="18" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="87" x14ac:dyDescent="0.35">
+      <c r="A12" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E17" s="23" t="s">
+      <c r="B12" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="7" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="B13" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="F13" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="23"/>
-    </row>
-    <row r="18" spans="1:7" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="24" t="s">
+      <c r="G13" s="18" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="7" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-    </row>
-    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="64" t="s">
-        <v>97</v>
-      </c>
-      <c r="B19" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
-    </row>
-    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="63" t="s">
-        <v>102</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>99</v>
-      </c>
+      <c r="B14" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="7" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="62"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="1:16" s="7" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="62"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="1:7" s="7" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="70"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="70"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="70"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="70"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="31"/>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
     </row>
-    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="64" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="66" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
-    </row>
-    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="B22" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="66" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
-    </row>
-    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="64" t="s">
-        <v>105</v>
-      </c>
-      <c r="B23" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="66" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="67"/>
-    </row>
-    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="64" t="s">
-        <v>107</v>
-      </c>
-      <c r="B24" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="66" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
+    <row r="21" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="70"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="70"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+    </row>
+    <row r="23" spans="1:7" s="7" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="70"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="1:7" s="7" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="70"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+    </row>
+    <row r="25" spans="1:7" s="7" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="71"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3885,7 +4279,7 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F24" xr:uid="{9EA43539-DEE0-4787-BD9C-557A3B5C94B1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F16" xr:uid="{9EA43539-DEE0-4787-BD9C-557A3B5C94B1}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3903,7 +4297,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3918,25 +4312,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" ht="28.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3964,43 +4358,45 @@
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" s="44" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="68" t="s">
-        <v>109</v>
+      <c r="A4" s="66" t="s">
+        <v>96</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" s="55"/>
+        <v>98</v>
+      </c>
+      <c r="D4" s="68" t="s">
+        <v>216</v>
+      </c>
       <c r="E4" s="23" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="O4" s="45"/>
       <c r="P4" s="45"/>
     </row>
     <row r="5" spans="1:16" s="44" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="68" t="s">
-        <v>118</v>
+      <c r="A5" s="66" t="s">
+        <v>105</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="D5" s="55" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="F5" s="23" t="s">
         <v>30</v>
@@ -4010,20 +4406,20 @@
       <c r="P5" s="45"/>
     </row>
     <row r="6" spans="1:16" s="44" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="68" t="s">
-        <v>123</v>
+      <c r="A6" s="66" t="s">
+        <v>110</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="D6" s="55" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="F6" s="23" t="s">
         <v>30</v>
@@ -4032,14 +4428,14 @@
       <c r="P6" s="45"/>
     </row>
     <row r="7" spans="1:16" s="44" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="68" t="s">
-        <v>127</v>
+      <c r="A7" s="66" t="s">
+        <v>114</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="D7" s="55"/>
       <c r="E7" s="23"/>
@@ -4047,17 +4443,29 @@
       <c r="G7" s="23"/>
       <c r="P7" s="45"/>
     </row>
-    <row r="8" spans="1:16" s="44" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="68"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
+    <row r="8" spans="1:16" s="44" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="66" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="72" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" s="68" t="s">
+        <v>220</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="F8" s="72" t="s">
+        <v>30</v>
+      </c>
       <c r="G8" s="23"/>
     </row>
     <row r="9" spans="1:16" s="44" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="68"/>
+      <c r="A9" s="66"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="55"/>
@@ -4066,13 +4474,13 @@
       <c r="G9" s="23"/>
     </row>
     <row r="10" spans="1:16" s="44" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="68"/>
+      <c r="A10" s="66"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="55"/>
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
-      <c r="G10" s="62"/>
+      <c r="G10" s="61"/>
     </row>
     <row r="11" spans="1:16" ht="12.5" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -4101,8 +4509,8 @@
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D11:D14"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4117,25 +4525,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" s="28" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4164,19 +4572,19 @@
     </row>
     <row r="4" spans="1:16" s="21" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="F4" s="20" t="s">
         <v>30</v>
@@ -4191,16 +4599,16 @@
     </row>
     <row r="5" spans="1:16" s="21" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="20"/>
@@ -4211,19 +4619,23 @@
     </row>
     <row r="6" spans="1:16" s="21" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
+        <v>224</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>30</v>
+      </c>
       <c r="G6" s="20"/>
       <c r="P6" s="22" t="s">
         <v>4</v>
@@ -4231,20 +4643,22 @@
     </row>
     <row r="7" spans="1:16" s="21" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="E7" s="20"/>
+        <v>223</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>222</v>
+      </c>
       <c r="F7" s="20" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G7" s="50"/>
       <c r="P7" s="22" t="s">
@@ -4253,87 +4667,133 @@
     </row>
     <row r="8" spans="1:16" s="21" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B8" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="C8" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="E8" s="20"/>
+      <c r="E8" s="20" t="s">
+        <v>247</v>
+      </c>
       <c r="F8" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="P8" s="22"/>
     </row>
     <row r="9" spans="1:16" s="21" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
+        <v>131</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>39</v>
+      </c>
       <c r="G9" s="23" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="21" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="D10" s="20"/>
+        <v>140</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>123</v>
+      </c>
       <c r="E10" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="F10" s="20"/>
+        <v>141</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>30</v>
+      </c>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="1:16" s="21" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+    <row r="11" spans="1:16" s="21" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>30</v>
+      </c>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="1:16" s="21" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+    <row r="12" spans="1:16" s="21" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>30</v>
+      </c>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="1:16" s="21" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+    <row r="13" spans="1:16" s="21" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>30</v>
+      </c>
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="1:16" s="21" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
@@ -4503,7 +4963,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4518,24 +4978,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
     </row>
     <row r="2" spans="1:7" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="76"/>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
+      <c r="A2" s="82"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
     </row>
     <row r="3" spans="1:7" s="15" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
@@ -4560,108 +5020,134 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="24" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="D4" s="23"/>
+        <v>143</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>235</v>
+      </c>
       <c r="E4" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>40</v>
+        <v>146</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>39</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-    </row>
-    <row r="6" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+        <v>148</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="47"/>
+    </row>
+    <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="24" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="D6" s="23"/>
+        <v>149</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>237</v>
+      </c>
       <c r="E6" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="F6" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" s="20" t="s">
         <v>30</v>
       </c>
       <c r="G6" s="23"/>
     </row>
-    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="24" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
+        <v>150</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>30</v>
+      </c>
       <c r="G7" s="23"/>
     </row>
-    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="24" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
+        <v>155</v>
+      </c>
+      <c r="D8" s="74" t="s">
+        <v>253</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>30</v>
+      </c>
       <c r="G8" s="23"/>
     </row>
     <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="24" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>130</v>
+        <v>254</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+        <v>157</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>259</v>
+      </c>
       <c r="F9" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9" s="50" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
@@ -4733,7 +5219,7 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F2" xr:uid="{0D250E04-2D09-4357-985A-E666B776A8EF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F2 F4:F8" xr:uid="{0D250E04-2D09-4357-985A-E666B776A8EF}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4749,7 +5235,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4764,24 +5250,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="76"/>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
+      <c r="A2" s="82"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
     </row>
     <row r="3" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
@@ -4808,100 +5294,132 @@
     </row>
     <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="30" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="18"/>
+        <v>162</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="G4" s="18"/>
     </row>
-    <row r="5" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="30" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="18"/>
+        <v>164</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="G5" s="18"/>
     </row>
-    <row r="6" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="30" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="18"/>
+        <v>165</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="30" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="18"/>
+        <v>168</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="30" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
+        <v>170</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>250</v>
+      </c>
       <c r="F8" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="30" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
+        <v>172</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="E9" s="73" t="s">
+        <v>252</v>
+      </c>
       <c r="F9" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
@@ -4936,7 +5454,7 @@
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F2 F4:F12" xr:uid="{8A108D50-398D-4367-BE11-C551A4B189B6}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
@@ -4956,7 +5474,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4973,28 +5491,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
     </row>
     <row r="2" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="78"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
+      <c r="A2" s="84"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
     </row>
     <row r="3" spans="1:9" s="37" customFormat="1" ht="31" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
@@ -5027,7 +5545,7 @@
     </row>
     <row r="4" spans="1:9" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="50" t="s">
         <v>34</v>
@@ -5041,23 +5559,23 @@
       <c r="E4" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="58" t="s">
         <v>33</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="H4" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4" s="50"/>
     </row>
     <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.25">
       <c r="A5" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="50" t="s">
         <v>45</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>46</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>37</v>
@@ -5066,25 +5584,25 @@
         <v>37</v>
       </c>
       <c r="E5" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="50" t="s">
+        <v>177</v>
+      </c>
+      <c r="H5" s="50" t="s">
         <v>47</v>
-      </c>
-      <c r="F5" s="59" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" s="50" t="s">
-        <v>49</v>
       </c>
       <c r="I5" s="50"/>
     </row>
     <row r="6" spans="1:9" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A6" s="50" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>37</v>
@@ -5093,165 +5611,179 @@
         <v>37</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="F6" s="58" t="s">
         <v>33</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H6" s="50" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I6" s="50"/>
     </row>
     <row r="7" spans="1:9" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A7" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>264</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="50" t="s">
+      <c r="H7" s="50" t="s">
         <v>76</v>
-      </c>
-      <c r="D7" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="50" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="50" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="57" t="s">
-        <v>80</v>
-      </c>
-      <c r="H7" s="50" t="s">
-        <v>81</v>
       </c>
       <c r="I7" s="50"/>
     </row>
     <row r="8" spans="1:9" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E8" s="50" t="s">
-        <v>114</v>
-      </c>
-      <c r="F8" s="59" t="s">
-        <v>115</v>
+        <v>101</v>
+      </c>
+      <c r="F8" s="58" t="s">
+        <v>102</v>
       </c>
       <c r="G8" s="50" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="H8" s="50" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="I8" s="50"/>
     </row>
     <row r="9" spans="1:9" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" s="50" t="s">
+        <v>246</v>
+      </c>
+      <c r="F9" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="G9" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="H9" s="50" t="s">
+        <v>139</v>
+      </c>
+      <c r="I9" s="50"/>
+    </row>
+    <row r="10" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="F10" s="74" t="s">
+        <v>235</v>
+      </c>
+      <c r="G10" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="H10" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="B9" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="C9" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="E9" s="50" t="s">
-        <v>152</v>
-      </c>
-      <c r="F9" s="50" t="s">
-        <v>153</v>
-      </c>
-      <c r="G9" s="50" t="s">
-        <v>154</v>
-      </c>
-      <c r="H9" s="50" t="s">
-        <v>155</v>
-      </c>
-      <c r="I9" s="50"/>
-    </row>
-    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.25">
-      <c r="A10" s="50" t="s">
-        <v>161</v>
-      </c>
-      <c r="B10" s="50" t="s">
+      <c r="I10" s="50"/>
+    </row>
+    <row r="11" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="A11" s="50" t="s">
         <v>158</v>
       </c>
-      <c r="C10" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="D10" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="50" t="s">
-        <v>162</v>
-      </c>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50" t="s">
-        <v>164</v>
-      </c>
-      <c r="H10" s="50" t="s">
-        <v>165</v>
-      </c>
-      <c r="I10" s="50"/>
-    </row>
-    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
-        <v>176</v>
-      </c>
       <c r="B11" s="50" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="F11" s="74" t="s">
+        <v>256</v>
+      </c>
+      <c r="G11" s="50" t="s">
+        <v>257</v>
+      </c>
+      <c r="H11" s="50" t="s">
+        <v>258</v>
+      </c>
+      <c r="I11" s="50"/>
+    </row>
+    <row r="12" spans="1:9" ht="58" x14ac:dyDescent="0.25">
+      <c r="A12" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12" s="50" t="s">
+        <v>260</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="50" t="s">
         <v>174</v>
       </c>
-      <c r="C11" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="D11" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="50" t="s">
-        <v>177</v>
-      </c>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-    </row>
-    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.25">
-      <c r="A12" s="50" t="s">
-        <v>191</v>
-      </c>
-      <c r="B12" s="50" t="s">
-        <v>192</v>
-      </c>
-      <c r="C12" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="50" t="s">
-        <v>193</v>
-      </c>
       <c r="E12" s="50" t="s">
-        <v>194</v>
-      </c>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="58"/>
+        <v>175</v>
+      </c>
+      <c r="F12" s="50" t="s">
+        <v>261</v>
+      </c>
+      <c r="G12" s="50" t="s">
+        <v>262</v>
+      </c>
+      <c r="H12" s="50" t="s">
+        <v>263</v>
+      </c>
       <c r="I12" s="50"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>